<commit_message>
Data with no ST generators is added. Thread mgmt can be done via config.hpp
</commit_message>
<xml_diff>
--- a/stocUCED/datasets/NREL118 Generator Calculations/Generators.xlsx
+++ b/stocUCED/datasets/NREL118 Generator Calculations/Generators.xlsx
@@ -1,29 +1,107 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/semihatakan/Documents/Coding Projects/Power Systems/tamingDuck/tamingDuck/stocUCED/datasets/NREL118 Generator Calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E587DE0D-80C8-7F44-BF26-FA8672085C76}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="460" windowWidth="25580" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Generators" sheetId="1" r:id="rId1"/>
+    <sheet name="System Characteristics" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
     <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Semih Atakan</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{D6644C4E-A1D3-6440-BE7E-FD4E61352CAD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Semih Atakan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Avg of first 15 days</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{3CF6DBE2-17AE-634F-8FB5-25A6BBE099F7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Semih Atakan:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Avg of first 15 days</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="409">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="415">
   <si>
     <t>GenID</t>
   </si>
@@ -1250,17 +1328,37 @@
   </si>
   <si>
     <t>CO2 (kg/h)</t>
+  </si>
+  <si>
+    <t>Max Capacity</t>
+  </si>
+  <si>
+    <t>January (avg)</t>
+  </si>
+  <si>
+    <t>July (avg)</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="0.000000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000000"/>
+    <numFmt numFmtId="166" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1395,8 +1493,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1576,8 +1687,20 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1692,8 +1815,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1736,13 +1879,30 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="1" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="34" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="1" fillId="33" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1782,6 +1942,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Percent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -4538,7 +4699,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V328"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -29473,4 +29636,318 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5E16CC-5294-AE4F-9367-6FECD8D006D4}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="8">
+        <v>114.92</v>
+      </c>
+      <c r="C3" s="9">
+        <f>B3/$B$12</f>
+        <v>2.8362618996142968E-3</v>
+      </c>
+      <c r="D3" s="8">
+        <v>114.92</v>
+      </c>
+      <c r="E3" s="10">
+        <f>D3/$B$12</f>
+        <v>2.8362618996142968E-3</v>
+      </c>
+      <c r="F3" s="8">
+        <v>114.92</v>
+      </c>
+      <c r="G3" s="10">
+        <f>F3/$B$12</f>
+        <v>2.8362618996142968E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="B4" s="8">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9">
+        <f t="shared" ref="C4:E11" si="0">B4/$B$12</f>
+        <v>4.9360631737109235E-4</v>
+      </c>
+      <c r="D4" s="8">
+        <v>20</v>
+      </c>
+      <c r="E4" s="10">
+        <f t="shared" si="0"/>
+        <v>4.9360631737109235E-4</v>
+      </c>
+      <c r="F4" s="8">
+        <v>20</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G11" si="1">F4/$B$12</f>
+        <v>4.9360631737109235E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B5" s="8">
+        <v>22</v>
+      </c>
+      <c r="C5" s="9">
+        <f t="shared" si="0"/>
+        <v>5.4296694910820162E-4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>22</v>
+      </c>
+      <c r="E5" s="10">
+        <f t="shared" si="0"/>
+        <v>5.4296694910820162E-4</v>
+      </c>
+      <c r="F5" s="8">
+        <v>22</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="1"/>
+        <v>5.4296694910820162E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="B6" s="8">
+        <v>18650.26999999999</v>
+      </c>
+      <c r="C6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.4602945546338279</v>
+      </c>
+      <c r="D6" s="8">
+        <v>18650.26999999999</v>
+      </c>
+      <c r="E6" s="10">
+        <f t="shared" si="0"/>
+        <v>0.4602945546338279</v>
+      </c>
+      <c r="F6" s="8">
+        <v>18650.26999999999</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="1"/>
+        <v>0.4602945546338279</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="8">
+        <v>16786.359999999993</v>
+      </c>
+      <c r="C7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.41429266708327034</v>
+      </c>
+      <c r="D7" s="8">
+        <v>16786.359999999993</v>
+      </c>
+      <c r="E7" s="10">
+        <f t="shared" si="0"/>
+        <v>0.41429266708327034</v>
+      </c>
+      <c r="F7" s="8">
+        <v>16786.359999999993</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="1"/>
+        <v>0.41429266708327034</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="B8" s="8">
+        <v>365.9</v>
+      </c>
+      <c r="C8" s="9">
+        <f t="shared" si="0"/>
+        <v>9.0305275763041346E-3</v>
+      </c>
+      <c r="D8" s="8">
+        <v>365.9</v>
+      </c>
+      <c r="E8" s="10">
+        <f t="shared" si="0"/>
+        <v>9.0305275763041346E-3</v>
+      </c>
+      <c r="F8" s="8">
+        <v>365.9</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="1"/>
+        <v>9.0305275763041346E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>385</v>
+      </c>
+      <c r="B9" s="8">
+        <v>35</v>
+      </c>
+      <c r="C9" s="9">
+        <f t="shared" si="0"/>
+        <v>8.6381105539941165E-4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>35</v>
+      </c>
+      <c r="E9" s="10">
+        <f t="shared" si="0"/>
+        <v>8.6381105539941165E-4</v>
+      </c>
+      <c r="F9" s="8">
+        <v>35</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="1"/>
+        <v>8.6381105539941165E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3445.7700000000004</v>
+      </c>
+      <c r="C10" s="9">
+        <f t="shared" si="0"/>
+        <v>8.5042692010389456E-2</v>
+      </c>
+      <c r="D10" s="8">
+        <v>643.6</v>
+      </c>
+      <c r="E10" s="10">
+        <f t="shared" si="0"/>
+        <v>1.5884251293001753E-2</v>
+      </c>
+      <c r="F10" s="11">
+        <v>1035.2</v>
+      </c>
+      <c r="G10" s="10">
+        <f t="shared" si="1"/>
+        <v>2.5549062987127742E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="7" t="s">
+        <v>388</v>
+      </c>
+      <c r="B11" s="8">
+        <v>1077.8999999999999</v>
+      </c>
+      <c r="C11" s="9">
+        <f t="shared" si="0"/>
+        <v>2.660291247471502E-2</v>
+      </c>
+      <c r="D11" s="8">
+        <v>151.30000000000001</v>
+      </c>
+      <c r="E11" s="10">
+        <f t="shared" si="0"/>
+        <v>3.7341317909123143E-3</v>
+      </c>
+      <c r="F11" s="11">
+        <v>440.9</v>
+      </c>
+      <c r="G11" s="10">
+        <f t="shared" si="1"/>
+        <v>1.0881551266445732E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="12" t="s">
+        <v>414</v>
+      </c>
+      <c r="B12" s="13">
+        <v>40518.119999999988</v>
+      </c>
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="13">
+        <v>40518.119999999988</v>
+      </c>
+      <c r="E12" s="14">
+        <v>1</v>
+      </c>
+      <c r="F12" s="13">
+        <v>40518.119999999988</v>
+      </c>
+      <c r="G12" s="14">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>